<commit_message>
Ammended tariff data to remove duplicates. Updated r script with a few minor updates.
</commit_message>
<xml_diff>
--- a/Tarriff data.xlsx
+++ b/Tarriff data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bevan.andrews\Documents\Applied micro project\ECOM185-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7269AA1-34A9-4E75-B50A-78B1FB6CA652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B918B9A-3926-4720-87BE-6E1DD6902AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="19785" xr2:uid="{7204E3AE-D80B-4234-80D8-DE876C5A1A66}"/>
   </bookViews>
   <sheets>
     <sheet name="indicators_mfn_applied_duty_14_" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators_mfn_applied_duty_14_!$U$1:$V$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators_mfn_applied_duty_14_!$A$1:$M$471</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,30 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3865" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3997" uniqueCount="254">
   <si>
     <t>reporter_name</t>
   </si>
@@ -804,9 +783,6 @@
     <t>Arms and ammunition; parts and accessoriesthereof</t>
   </si>
   <si>
-    <t>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminatedname-plates and the like; prefabricated buildings</t>
-  </si>
-  <si>
     <t>Toys, games and sports requisites; parts and accessories thereof</t>
   </si>
   <si>
@@ -820,6 +796,9 @@
   </si>
   <si>
     <t>MFN</t>
+  </si>
+  <si>
+    <t>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminated name-plates and the like; prefabricated buildings</t>
   </si>
 </sst>
 </file>
@@ -1369,10 +1348,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1690,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA24C76-3D75-422A-B7CD-C37446D883C9}">
-  <dimension ref="A1:R471"/>
+  <dimension ref="A1:P471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,6 +1680,7 @@
     <col min="15" max="15" width="44" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="33" customWidth="1"/>
     <col min="17" max="17" width="19.28515625" customWidth="1"/>
+    <col min="20" max="20" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1745,13 +1721,13 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>251</v>
+      </c>
+      <c r="O1" t="s">
         <v>252</v>
       </c>
-      <c r="O1" t="s">
-        <v>253</v>
-      </c>
       <c r="P1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1792,12 +1768,11 @@
         <v>8.2163839285714302E-2</v>
       </c>
       <c r="M2" t="str">
-        <f>INDEX($P$2:$P$90,MATCH(I2,$O$2:$O$90,0))</f>
+        <f>INDEX($P$2:$P$56,MATCH(I2,$O$2:$O$56,0))</f>
         <v>Fish and crustaceans, molluscs and other aquatic invertebrates</v>
       </c>
-      <c r="O2" t="str" cm="1">
-        <f t="array" ref="O2:O90">_xlfn.UNIQUE(I2:I471)</f>
-        <v>Fish and fish products</v>
+      <c r="O2" t="s">
+        <v>19</v>
       </c>
       <c r="P2" t="s">
         <v>203</v>
@@ -1844,11 +1819,11 @@
         <f t="shared" ref="M3:M66" si="0">INDEX($P$2:$P$90,MATCH(I3,$O$2:$O$90,0))</f>
         <v>Fish and crustaceans, molluscs and other aquatic invertebrates</v>
       </c>
-      <c r="O3" t="str">
-        <v>Other agricultural products</v>
+      <c r="O3" t="s">
+        <v>21</v>
       </c>
       <c r="P3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1892,8 +1867,8 @@
         <f t="shared" si="0"/>
         <v>Fish and crustaceans, molluscs and other aquatic invertebrates</v>
       </c>
-      <c r="O4" t="str">
-        <v>Sugars and sugar confectionery</v>
+      <c r="O4" t="s">
+        <v>23</v>
       </c>
       <c r="P4" t="s">
         <v>23</v>
@@ -1940,8 +1915,8 @@
         <f t="shared" si="0"/>
         <v>Fish and crustaceans, molluscs and other aquatic invertebrates</v>
       </c>
-      <c r="O5" t="str">
-        <v>Electrical machinery and electronic equipment</v>
+      <c r="O5" t="s">
+        <v>25</v>
       </c>
       <c r="P5" t="s">
         <v>240</v>
@@ -1988,8 +1963,8 @@
         <f t="shared" si="0"/>
         <v>Fish and crustaceans, molluscs and other aquatic invertebrates</v>
       </c>
-      <c r="O6" t="str">
-        <v>Live animals and meat</v>
+      <c r="O6" t="s">
+        <v>27</v>
       </c>
       <c r="P6" t="s">
         <v>201</v>
@@ -2036,8 +2011,8 @@
         <f t="shared" si="0"/>
         <v>Other products</v>
       </c>
-      <c r="O7" t="str">
-        <v>Fruits and vegetables</v>
+      <c r="O7" t="s">
+        <v>29</v>
       </c>
       <c r="P7" t="s">
         <v>207</v>
@@ -2084,8 +2059,8 @@
         <f t="shared" si="0"/>
         <v>Other products</v>
       </c>
-      <c r="O8" t="str">
-        <v>Cotton, silk and wool</v>
+      <c r="O8" t="s">
+        <v>31</v>
       </c>
       <c r="P8" t="s">
         <v>186</v>
@@ -2132,8 +2107,8 @@
         <f t="shared" si="0"/>
         <v>Other products</v>
       </c>
-      <c r="O9" t="str">
-        <v>Petroleum</v>
+      <c r="O9" t="s">
+        <v>33</v>
       </c>
       <c r="P9" t="s">
         <v>218</v>
@@ -2180,8 +2155,8 @@
         <f t="shared" si="0"/>
         <v>Other products</v>
       </c>
-      <c r="O10" t="str">
-        <v>Plastics</v>
+      <c r="O10" t="s">
+        <v>36</v>
       </c>
       <c r="P10" t="s">
         <v>223</v>
@@ -2228,8 +2203,8 @@
         <f t="shared" si="0"/>
         <v>Other products</v>
       </c>
-      <c r="O11" t="str">
-        <v>Non-alcoholic beverages, including juices</v>
+      <c r="O11" t="s">
+        <v>38</v>
       </c>
       <c r="P11" t="s">
         <v>215</v>
@@ -2276,8 +2251,8 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O12" t="str">
-        <v>Dairy products</v>
+      <c r="O12" t="s">
+        <v>40</v>
       </c>
       <c r="P12" t="s">
         <v>204</v>
@@ -2324,8 +2299,8 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O13" t="str">
-        <v>Other textile products</v>
+      <c r="O13" t="s">
+        <v>42</v>
       </c>
       <c r="P13" t="s">
         <v>233</v>
@@ -2372,8 +2347,8 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O14" t="str">
-        <v>Metal products</v>
+      <c r="O14" t="s">
+        <v>44</v>
       </c>
       <c r="P14" t="s">
         <v>238</v>
@@ -2420,11 +2395,11 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O15" t="str">
-        <v>Other minerals</v>
+      <c r="O15" t="s">
+        <v>48</v>
       </c>
       <c r="P15" t="s">
-        <v>218</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2468,11 +2443,11 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O16" t="str">
-        <v>Mechanical, office and computing machinery</v>
+      <c r="O16" t="s">
+        <v>50</v>
       </c>
       <c r="P16" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -2516,11 +2491,11 @@
         <f t="shared" si="0"/>
         <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
       </c>
-      <c r="O17" t="str">
-        <v>Rubber, leather and footwear</v>
+      <c r="O17" t="s">
+        <v>54</v>
       </c>
       <c r="P17" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -2564,11 +2539,11 @@
         <f t="shared" si="0"/>
         <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
       </c>
-      <c r="O18" t="str">
-        <v>Other manufactures</v>
+      <c r="O18" t="s">
+        <v>56</v>
       </c>
       <c r="P18" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2612,11 +2587,11 @@
         <f t="shared" si="0"/>
         <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
       </c>
-      <c r="O19" t="str">
-        <v>Clothing</v>
+      <c r="O19" t="s">
+        <v>59</v>
       </c>
       <c r="P19" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2660,11 +2635,11 @@
         <f t="shared" si="0"/>
         <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
       </c>
-      <c r="O20" t="str">
-        <v>Minerals and metals</v>
+      <c r="O20" t="s">
+        <v>61</v>
       </c>
       <c r="P20" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -2708,11 +2683,11 @@
         <f t="shared" si="0"/>
         <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
       </c>
-      <c r="O21" t="str">
-        <v>Cocoa</v>
+      <c r="O21" t="s">
+        <v>63</v>
       </c>
       <c r="P21" t="s">
-        <v>212</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2756,11 +2731,11 @@
         <f t="shared" si="0"/>
         <v>Live animals</v>
       </c>
-      <c r="O22" t="str">
-        <v>Wood, paper, furniture</v>
+      <c r="O22" t="s">
+        <v>65</v>
       </c>
       <c r="P22" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2804,11 +2779,11 @@
         <f t="shared" si="0"/>
         <v>Live animals</v>
       </c>
-      <c r="O23" t="str">
-        <v>Cereals and food preparations</v>
+      <c r="O23" t="s">
+        <v>67</v>
       </c>
       <c r="P23" t="s">
-        <v>117</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -2852,11 +2827,11 @@
         <f t="shared" si="0"/>
         <v>Live animals</v>
       </c>
-      <c r="O24" t="str">
-        <v>Textiles</v>
+      <c r="O24" t="s">
+        <v>71</v>
       </c>
       <c r="P24" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2900,11 +2875,11 @@
         <f t="shared" si="0"/>
         <v>Live animals</v>
       </c>
-      <c r="O25" t="str">
-        <v>Ships and floating structures</v>
+      <c r="O25" t="s">
+        <v>73</v>
       </c>
       <c r="P25" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2948,11 +2923,11 @@
         <f t="shared" si="0"/>
         <v>Live animals</v>
       </c>
-      <c r="O26" t="str">
-        <v>Computers and office machinery</v>
+      <c r="O26" t="s">
+        <v>75</v>
       </c>
       <c r="P26" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2996,11 +2971,11 @@
         <f t="shared" si="0"/>
         <v>Edible vegetables and certain roots and tubers</v>
       </c>
-      <c r="O27" t="str">
-        <v>Audio-visual devices</v>
+      <c r="O27" t="s">
+        <v>79</v>
       </c>
       <c r="P27" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -3044,11 +3019,11 @@
         <f t="shared" si="0"/>
         <v>Edible vegetables and certain roots and tubers</v>
       </c>
-      <c r="O28" t="str">
-        <v>Oilseeds</v>
+      <c r="O28" t="s">
+        <v>81</v>
       </c>
       <c r="P28" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -3092,11 +3067,11 @@
         <f t="shared" si="0"/>
         <v>Edible vegetables and certain roots and tubers</v>
       </c>
-      <c r="O29" t="str">
-        <v>Furniture</v>
+      <c r="O29" t="s">
+        <v>87</v>
       </c>
       <c r="P29" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -3140,11 +3115,11 @@
         <f t="shared" si="0"/>
         <v>Edible vegetables and certain roots and tubers</v>
       </c>
-      <c r="O30" t="str">
-        <v>Crude oils</v>
+      <c r="O30" t="s">
+        <v>91</v>
       </c>
       <c r="P30" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -3188,11 +3163,11 @@
         <f t="shared" si="0"/>
         <v>Edible vegetables and certain roots and tubers</v>
       </c>
-      <c r="O31" t="str">
-        <v>Man-made fibre, yarn and fabrics</v>
+      <c r="O31" t="s">
+        <v>93</v>
       </c>
       <c r="P31" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3236,11 +3211,11 @@
         <f t="shared" si="0"/>
         <v>Cotton</v>
       </c>
-      <c r="O32" t="str">
-        <v>Food preparations</v>
+      <c r="O32" t="s">
+        <v>95</v>
       </c>
       <c r="P32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -3284,11 +3259,11 @@
         <f t="shared" si="0"/>
         <v>Cotton</v>
       </c>
-      <c r="O33" t="str">
-        <v>Measuring instruments</v>
+      <c r="O33" t="s">
+        <v>97</v>
       </c>
       <c r="P33" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -3332,11 +3307,11 @@
         <f t="shared" si="0"/>
         <v>Cotton</v>
       </c>
-      <c r="O34" t="str">
-        <v>Vegetables</v>
+      <c r="O34" t="s">
+        <v>99</v>
       </c>
       <c r="P34" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3380,11 +3355,11 @@
         <f t="shared" si="0"/>
         <v>Cotton</v>
       </c>
-      <c r="O35" t="str">
-        <v>Tobacco</v>
+      <c r="O35" t="s">
+        <v>101</v>
       </c>
       <c r="P35" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3428,11 +3403,11 @@
         <f t="shared" si="0"/>
         <v>Cotton</v>
       </c>
-      <c r="O36" t="str">
-        <v>Rubber and rubber products</v>
+      <c r="O36" t="s">
+        <v>103</v>
       </c>
       <c r="P36" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -3476,11 +3451,11 @@
         <f t="shared" si="0"/>
         <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
       </c>
-      <c r="O37" t="str">
-        <v>Pharmaceuticals</v>
+      <c r="O37" t="s">
+        <v>107</v>
       </c>
       <c r="P37" t="s">
-        <v>220</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3524,11 +3499,11 @@
         <f t="shared" si="0"/>
         <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
       </c>
-      <c r="O38" t="str">
-        <v>Arms and ammunition</v>
+      <c r="O38" t="s">
+        <v>109</v>
       </c>
       <c r="P38" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3572,11 +3547,11 @@
         <f t="shared" si="0"/>
         <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
       </c>
-      <c r="O39" t="str">
-        <v>Vegetable fats and oils</v>
+      <c r="O39" t="s">
+        <v>111</v>
       </c>
       <c r="P39" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3620,11 +3595,11 @@
         <f t="shared" si="0"/>
         <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
       </c>
-      <c r="O40" t="str">
-        <v>Bicycles, motorcycles and other transport equipment</v>
+      <c r="O40" t="s">
+        <v>190</v>
       </c>
       <c r="P40" t="s">
-        <v>242</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -3668,11 +3643,11 @@
         <f t="shared" si="0"/>
         <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
       </c>
-      <c r="O41" t="str">
-        <v>Railway vehicles</v>
+      <c r="O41" t="s">
+        <v>119</v>
       </c>
       <c r="P41" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -3716,11 +3691,11 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O42" t="str">
-        <v>Clocks and watches</v>
+      <c r="O42" t="s">
+        <v>178</v>
       </c>
       <c r="P42" t="s">
-        <v>246</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -3764,11 +3739,11 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O43" t="str">
-        <v>Natural fibre, yarn and fabrics</v>
+      <c r="O43" t="s">
+        <v>131</v>
       </c>
       <c r="P43" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3812,11 +3787,11 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O44" t="str">
-        <v>Wood and wood products</v>
+      <c r="O44" t="s">
+        <v>133</v>
       </c>
       <c r="P44" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -3860,11 +3835,11 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O45" t="str">
-        <v>Recreational and sports products</v>
+      <c r="O45" t="s">
+        <v>145</v>
       </c>
       <c r="P45" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3908,11 +3883,11 @@
         <f t="shared" si="0"/>
         <v>Sugars and sugar confectionery</v>
       </c>
-      <c r="O46" t="str">
-        <v>Inorganic chemicals</v>
+      <c r="O46" t="s">
+        <v>147</v>
       </c>
       <c r="P46" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3956,11 +3931,11 @@
         <f t="shared" si="0"/>
         <v>Plastics and plastic products</v>
       </c>
-      <c r="O47" t="str">
-        <v>Aircraft</v>
+      <c r="O47" t="s">
+        <v>155</v>
       </c>
       <c r="P47" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4004,11 +3979,11 @@
         <f t="shared" si="0"/>
         <v>Plastics and plastic products</v>
       </c>
-      <c r="O48" t="str">
-        <v>Non-ferrous metals</v>
+      <c r="O48" t="s">
+        <v>158</v>
       </c>
       <c r="P48" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4052,11 +4027,11 @@
         <f t="shared" si="0"/>
         <v>Plastics and plastic products</v>
       </c>
-      <c r="O49" t="str">
-        <v>Motor vehicles</v>
+      <c r="O49" t="s">
+        <v>164</v>
       </c>
       <c r="P49" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -4100,11 +4075,11 @@
         <f t="shared" si="0"/>
         <v>Plastics and plastic products</v>
       </c>
-      <c r="O50" t="str">
-        <v>Cereals</v>
+      <c r="O50" t="s">
+        <v>172</v>
       </c>
       <c r="P50" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -4148,11 +4123,11 @@
         <f t="shared" si="0"/>
         <v>Plastics and plastic products</v>
       </c>
-      <c r="O51" t="str">
-        <v>Fertilisers</v>
+      <c r="O51" t="s">
+        <v>174</v>
       </c>
       <c r="P51" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -4196,11 +4171,11 @@
         <f t="shared" si="0"/>
         <v>Beverages, spirits and vinegar</v>
       </c>
-      <c r="O52" t="str">
-        <v>Non-metallic mineral products</v>
+      <c r="O52" t="s">
+        <v>176</v>
       </c>
       <c r="P52" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -4244,11 +4219,11 @@
         <f t="shared" si="0"/>
         <v>Beverages, spirits and vinegar</v>
       </c>
-      <c r="O53" t="str">
-        <v>Transport equipment</v>
+      <c r="O53" t="s">
+        <v>180</v>
       </c>
       <c r="P53" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4292,11 +4267,11 @@
         <f t="shared" si="0"/>
         <v>Beverages, spirits and vinegar</v>
       </c>
-      <c r="O54" t="str">
-        <v>Chemicals</v>
+      <c r="O54" t="s">
+        <v>192</v>
       </c>
       <c r="P54" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4340,11 +4315,11 @@
         <f t="shared" si="0"/>
         <v>Beverages, spirits and vinegar</v>
       </c>
-      <c r="O55" t="str">
-        <v>Beverages and tobacco</v>
+      <c r="O55" t="s">
+        <v>194</v>
       </c>
       <c r="P55" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4388,11 +4363,11 @@
         <f t="shared" si="0"/>
         <v>Beverages, spirits and vinegar</v>
       </c>
-      <c r="O56" t="str">
-        <v>Oilseeds, fats and oils</v>
+      <c r="O56" t="s">
+        <v>198</v>
       </c>
       <c r="P56" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4436,12 +4411,6 @@
         <f t="shared" si="0"/>
         <v>Dairy produce; birds' eggs; natural honey; edible products of animal origin, not elsewhere specified or included</v>
       </c>
-      <c r="O57" t="str">
-        <v>Coffee, tea, cocoa and spices</v>
-      </c>
-      <c r="P57" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -4484,12 +4453,6 @@
         <f t="shared" si="0"/>
         <v>Dairy produce; birds' eggs; natural honey; edible products of animal origin, not elsewhere specified or included</v>
       </c>
-      <c r="O58" t="str">
-        <v>Jewellery and related products</v>
-      </c>
-      <c r="P58" t="s">
-        <v>235</v>
-      </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -4532,12 +4495,6 @@
         <f t="shared" si="0"/>
         <v>Dairy produce; birds' eggs; natural honey; edible products of animal origin, not elsewhere specified or included</v>
       </c>
-      <c r="O59" t="str">
-        <v>Electronic components</v>
-      </c>
-      <c r="P59" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -4580,12 +4537,6 @@
         <f t="shared" si="0"/>
         <v>Dairy produce; birds' eggs; natural honey; edible products of animal origin, not elsewhere specified or included</v>
       </c>
-      <c r="O60" t="str">
-        <v>Spices</v>
-      </c>
-      <c r="P60" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -4628,12 +4579,6 @@
         <f t="shared" si="0"/>
         <v>Dairy produce; birds' eggs; natural honey; edible products of animal origin, not elsewhere specified or included</v>
       </c>
-      <c r="O61" t="str">
-        <v>Alcohols</v>
-      </c>
-      <c r="P61" t="s">
-        <v>215</v>
-      </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -4676,12 +4621,6 @@
         <f t="shared" si="0"/>
         <v>Other made up textile articles; sets; worn clothing and worn textile articles; rags</v>
       </c>
-      <c r="O62" t="str">
-        <v>Animal fats and oils</v>
-      </c>
-      <c r="P62" t="s">
-        <v>211</v>
-      </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -4724,12 +4663,6 @@
         <f t="shared" si="0"/>
         <v>Other made up textile articles; sets; worn clothing and worn textile articles; rags</v>
       </c>
-      <c r="O63" t="str">
-        <v>Machinery for specialized industries</v>
-      </c>
-      <c r="P63" t="s">
-        <v>239</v>
-      </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -4772,14 +4705,8 @@
         <f t="shared" si="0"/>
         <v>Other made up textile articles; sets; worn clothing and worn textile articles; rags</v>
       </c>
-      <c r="O64" t="str">
-        <v>Residues of food processing industry</v>
-      </c>
-      <c r="P64" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -4820,17 +4747,8 @@
         <f t="shared" si="0"/>
         <v>Other made up textile articles; sets; worn clothing and worn textile articles; rags</v>
       </c>
-      <c r="O65" t="str">
-        <v>Silk and wool</v>
-      </c>
-      <c r="P65" t="s">
-        <v>228</v>
-      </c>
-      <c r="R65" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -4871,14 +4789,8 @@
         <f t="shared" si="0"/>
         <v>Other made up textile articles; sets; worn clothing and worn textile articles; rags</v>
       </c>
-      <c r="O66" t="str">
-        <v>Power generating machinery</v>
-      </c>
-      <c r="P66" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -4919,14 +4831,8 @@
         <f t="shared" ref="M67:M130" si="1">INDEX($P$2:$P$90,MATCH(I67,$O$2:$O$90,0))</f>
         <v>Miscellaneous articles of base metal</v>
       </c>
-      <c r="O67" t="str">
-        <v>Mineral fuels, other than petroleum oils</v>
-      </c>
-      <c r="P67" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -4967,14 +4873,8 @@
         <f t="shared" si="1"/>
         <v>Miscellaneous articles of base metal</v>
       </c>
-      <c r="O68" t="str">
-        <v>Organic chemicals</v>
-      </c>
-      <c r="P68" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -5015,14 +4915,8 @@
         <f t="shared" si="1"/>
         <v>Miscellaneous articles of base metal</v>
       </c>
-      <c r="O69" t="str">
-        <v>Fruit and vegetable preparations</v>
-      </c>
-      <c r="P69" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -5063,14 +4957,8 @@
         <f t="shared" si="1"/>
         <v>Miscellaneous articles of base metal</v>
       </c>
-      <c r="O70" t="str">
-        <v>Plants and vegetal material</v>
-      </c>
-      <c r="P70" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -5111,14 +4999,8 @@
         <f t="shared" si="1"/>
         <v>Miscellaneous articles of base metal</v>
       </c>
-      <c r="O71" t="str">
-        <v>Semiconductors</v>
-      </c>
-      <c r="P71" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -5155,18 +5037,12 @@
       <c r="L72">
         <v>0.91015904761904798</v>
       </c>
-      <c r="M72" t="str">
+      <c r="M72" t="e">
         <f t="shared" si="1"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
-      </c>
-      <c r="O72" t="str">
-        <v>Optical and photographic products</v>
-      </c>
-      <c r="P72" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -5203,18 +5079,12 @@
       <c r="L73">
         <v>0.91015904761904798</v>
       </c>
-      <c r="M73" t="str">
+      <c r="M73" t="e">
         <f t="shared" si="1"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
-      </c>
-      <c r="O73" t="str">
-        <v>Pulp, paper and printed matter</v>
-      </c>
-      <c r="P73" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -5251,18 +5121,12 @@
       <c r="L74">
         <v>0.91015904761904798</v>
       </c>
-      <c r="M74" t="str">
+      <c r="M74" t="e">
         <f t="shared" si="1"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
-      </c>
-      <c r="O74" t="str">
-        <v>General industrial machinery</v>
-      </c>
-      <c r="P74" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -5299,18 +5163,12 @@
       <c r="L75">
         <v>0.91015904761904798</v>
       </c>
-      <c r="M75" t="str">
+      <c r="M75" t="e">
         <f t="shared" si="1"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
-      </c>
-      <c r="O75" t="str">
-        <v>Petroleum oils, other than crude</v>
-      </c>
-      <c r="P75" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -5347,18 +5205,12 @@
       <c r="L76">
         <v>0.91015904761904798</v>
       </c>
-      <c r="M76" t="str">
+      <c r="M76" t="e">
         <f t="shared" si="1"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
-      </c>
-      <c r="O76" t="str">
-        <v>Other products of animal origin</v>
-      </c>
-      <c r="P76" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -5399,14 +5251,8 @@
         <f t="shared" si="1"/>
         <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
       </c>
-      <c r="O77" t="str">
-        <v>Leather and leather products</v>
-      </c>
-      <c r="P77" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -5447,14 +5293,8 @@
         <f t="shared" si="1"/>
         <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
       </c>
-      <c r="O78" t="str">
-        <v>Footwear</v>
-      </c>
-      <c r="P78" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -5495,14 +5335,8 @@
         <f t="shared" si="1"/>
         <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
       </c>
-      <c r="O79" t="str">
-        <v>Chemicals from agricultural origin</v>
-      </c>
-      <c r="P79" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -5543,14 +5377,8 @@
         <f t="shared" si="1"/>
         <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
       </c>
-      <c r="O80" t="str">
-        <v>Meat</v>
-      </c>
-      <c r="P80" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -5591,14 +5419,8 @@
         <f t="shared" si="1"/>
         <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
       </c>
-      <c r="O81" t="str">
-        <v>Medical equipment</v>
-      </c>
-      <c r="P81" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -5639,14 +5461,8 @@
         <f t="shared" si="1"/>
         <v>Rubber and articles thereof</v>
       </c>
-      <c r="O82" t="str">
-        <v>Electrical machinery</v>
-      </c>
-      <c r="P82" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -5687,14 +5503,8 @@
         <f t="shared" si="1"/>
         <v>Rubber and articles thereof</v>
       </c>
-      <c r="O83" t="str">
-        <v>Cotton</v>
-      </c>
-      <c r="P83" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -5735,14 +5545,8 @@
         <f t="shared" si="1"/>
         <v>Rubber and articles thereof</v>
       </c>
-      <c r="O84" t="str">
-        <v>Live animals, excluding fish</v>
-      </c>
-      <c r="P84" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -5783,14 +5587,8 @@
         <f t="shared" si="1"/>
         <v>Rubber and articles thereof</v>
       </c>
-      <c r="O85" t="str">
-        <v>Iron and steel</v>
-      </c>
-      <c r="P85" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -5831,14 +5629,8 @@
         <f t="shared" si="1"/>
         <v>Rubber and articles thereof</v>
       </c>
-      <c r="O86" t="str">
-        <v>Domestic appliances</v>
-      </c>
-      <c r="P86" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -5875,18 +5667,12 @@
       <c r="L87">
         <v>0.20752294617563699</v>
       </c>
-      <c r="M87" t="str">
+      <c r="M87" t="e">
         <f t="shared" si="1"/>
-        <v>Other products</v>
-      </c>
-      <c r="O87" t="str">
-        <v>Fruits</v>
-      </c>
-      <c r="P87" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -5923,18 +5709,12 @@
       <c r="L88">
         <v>0.20811303116147301</v>
       </c>
-      <c r="M88" t="str">
+      <c r="M88" t="e">
         <f t="shared" si="1"/>
-        <v>Other products</v>
-      </c>
-      <c r="O88" t="str">
-        <v>Coffee, tea, mate</v>
-      </c>
-      <c r="P88" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -5971,18 +5751,12 @@
       <c r="L89">
         <v>0.20752294617563699</v>
       </c>
-      <c r="M89" t="str">
+      <c r="M89" t="e">
         <f t="shared" si="1"/>
-        <v>Other products</v>
-      </c>
-      <c r="O89" t="str">
-        <v>Other chemical products</v>
-      </c>
-      <c r="P89" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -6019,18 +5793,12 @@
       <c r="L90">
         <v>0.20811303116147301</v>
       </c>
-      <c r="M90" t="str">
+      <c r="M90" t="e">
         <f t="shared" si="1"/>
-        <v>Other products</v>
-      </c>
-      <c r="O90" t="str">
-        <v>Telecommunication equipment</v>
-      </c>
-      <c r="P90" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -6067,12 +5835,12 @@
       <c r="L91">
         <v>0.20811303116147301</v>
       </c>
-      <c r="M91" t="str">
+      <c r="M91" t="e">
         <f t="shared" si="1"/>
-        <v>Other products</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -6114,7 +5882,7 @@
         <v>Articles of apparel and clothing accessories, not knitted or crocheted</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>12</v>
       </c>
@@ -6156,7 +5924,7 @@
         <v>Articles of apparel and clothing accessories, not knitted or crocheted</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>12</v>
       </c>
@@ -6198,7 +5966,7 @@
         <v>Articles of apparel and clothing accessories, not knitted or crocheted</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>12</v>
       </c>
@@ -6240,7 +6008,7 @@
         <v>Articles of apparel and clothing accessories, not knitted or crocheted</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -7789,9 +7557,9 @@
       <c r="L132">
         <v>0.87413793103448301</v>
       </c>
-      <c r="M132" t="str">
+      <c r="M132" t="e">
         <f t="shared" si="2"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -7831,9 +7599,9 @@
       <c r="L133">
         <v>0.87413793103448301</v>
       </c>
-      <c r="M133" t="str">
+      <c r="M133" t="e">
         <f t="shared" si="2"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -7873,9 +7641,9 @@
       <c r="L134">
         <v>0.87413793103448301</v>
       </c>
-      <c r="M134" t="str">
+      <c r="M134" t="e">
         <f t="shared" si="2"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -7915,9 +7683,9 @@
       <c r="L135">
         <v>0.87413793103448301</v>
       </c>
-      <c r="M135" t="str">
+      <c r="M135" t="e">
         <f t="shared" si="2"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -7957,9 +7725,9 @@
       <c r="L136">
         <v>0.87413793103448301</v>
       </c>
-      <c r="M136" t="str">
+      <c r="M136" t="e">
         <f t="shared" si="2"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -8421,7 +8189,7 @@
       </c>
       <c r="M147" t="str">
         <f t="shared" si="2"/>
-        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminatedname-plates and the like; prefabricated buildings</v>
+        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminated name-plates and the like; prefabricated buildings</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -8463,7 +8231,7 @@
       </c>
       <c r="M148" t="str">
         <f t="shared" si="2"/>
-        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminatedname-plates and the like; prefabricated buildings</v>
+        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminated name-plates and the like; prefabricated buildings</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -8505,7 +8273,7 @@
       </c>
       <c r="M149" t="str">
         <f t="shared" si="2"/>
-        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminatedname-plates and the like; prefabricated buildings</v>
+        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminated name-plates and the like; prefabricated buildings</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -8547,7 +8315,7 @@
       </c>
       <c r="M150" t="str">
         <f t="shared" si="2"/>
-        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminatedname-plates and the like; prefabricated buildings</v>
+        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminated name-plates and the like; prefabricated buildings</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -8589,7 +8357,7 @@
       </c>
       <c r="M151" t="str">
         <f t="shared" si="2"/>
-        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminatedname-plates and the like; prefabricated buildings</v>
+        <v>Furniture; medical and surgical furniture; bedding, mattresses, mattress supports,cushions and similar stuffed furnishings; lamps and lighting fittings, not elsewhere specified; illuminated signs, illuminated name-plates and the like; prefabricated buildings</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
@@ -8629,9 +8397,9 @@
       <c r="L152">
         <v>1</v>
       </c>
-      <c r="M152" t="str">
+      <c r="M152" t="e">
         <f t="shared" si="2"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -8671,9 +8439,9 @@
       <c r="L153">
         <v>1</v>
       </c>
-      <c r="M153" t="str">
+      <c r="M153" t="e">
         <f t="shared" si="2"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -8713,9 +8481,9 @@
       <c r="L154">
         <v>1</v>
       </c>
-      <c r="M154" t="str">
+      <c r="M154" t="e">
         <f t="shared" si="2"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -8755,9 +8523,9 @@
       <c r="L155">
         <v>1</v>
       </c>
-      <c r="M155" t="str">
+      <c r="M155" t="e">
         <f t="shared" si="2"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
@@ -8797,9 +8565,9 @@
       <c r="L156">
         <v>1</v>
       </c>
-      <c r="M156" t="str">
+      <c r="M156" t="e">
         <f t="shared" si="2"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
@@ -9259,9 +9027,9 @@
       <c r="L167">
         <v>0.29021111111111098</v>
       </c>
-      <c r="M167" t="str">
+      <c r="M167" t="e">
         <f t="shared" si="2"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -9301,9 +9069,9 @@
       <c r="L168">
         <v>0.29021111111111098</v>
       </c>
-      <c r="M168" t="str">
+      <c r="M168" t="e">
         <f t="shared" si="2"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -9343,9 +9111,9 @@
       <c r="L169">
         <v>0.29021111111111098</v>
       </c>
-      <c r="M169" t="str">
+      <c r="M169" t="e">
         <f t="shared" si="2"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -9385,9 +9153,9 @@
       <c r="L170">
         <v>0.29021111111111098</v>
       </c>
-      <c r="M170" t="str">
+      <c r="M170" t="e">
         <f t="shared" si="2"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -9427,9 +9195,9 @@
       <c r="L171">
         <v>0.29021111111111098</v>
       </c>
-      <c r="M171" t="str">
+      <c r="M171" t="e">
         <f t="shared" si="2"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
@@ -9469,9 +9237,9 @@
       <c r="L172">
         <v>0.144279104477612</v>
       </c>
-      <c r="M172" t="str">
+      <c r="M172" t="e">
         <f t="shared" si="2"/>
-        <v>Edible vegetables and certain roots and tubers</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -9511,9 +9279,9 @@
       <c r="L173">
         <v>0.144279104477612</v>
       </c>
-      <c r="M173" t="str">
+      <c r="M173" t="e">
         <f t="shared" si="2"/>
-        <v>Edible vegetables and certain roots and tubers</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -9553,9 +9321,9 @@
       <c r="L174">
         <v>0.144279104477612</v>
       </c>
-      <c r="M174" t="str">
+      <c r="M174" t="e">
         <f t="shared" si="2"/>
-        <v>Edible vegetables and certain roots and tubers</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
@@ -9595,9 +9363,9 @@
       <c r="L175">
         <v>0.144279104477612</v>
       </c>
-      <c r="M175" t="str">
+      <c r="M175" t="e">
         <f t="shared" si="2"/>
-        <v>Edible vegetables and certain roots and tubers</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
@@ -9637,9 +9405,9 @@
       <c r="L176">
         <v>0.144279104477612</v>
       </c>
-      <c r="M176" t="str">
+      <c r="M176" t="e">
         <f t="shared" si="2"/>
-        <v>Edible vegetables and certain roots and tubers</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
@@ -9889,9 +9657,9 @@
       <c r="L182">
         <v>0.34705882352941197</v>
       </c>
-      <c r="M182" t="str">
+      <c r="M182" t="e">
         <f t="shared" si="2"/>
-        <v>Rubber and articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
@@ -9931,9 +9699,9 @@
       <c r="L183">
         <v>0.34705882352941197</v>
       </c>
-      <c r="M183" t="str">
+      <c r="M183" t="e">
         <f t="shared" si="2"/>
-        <v>Rubber and articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
@@ -9973,9 +9741,9 @@
       <c r="L184">
         <v>0.34705882352941197</v>
       </c>
-      <c r="M184" t="str">
+      <c r="M184" t="e">
         <f t="shared" si="2"/>
-        <v>Rubber and articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
@@ -10015,9 +9783,9 @@
       <c r="L185">
         <v>0.34705882352941197</v>
       </c>
-      <c r="M185" t="str">
+      <c r="M185" t="e">
         <f t="shared" si="2"/>
-        <v>Rubber and articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
@@ -10057,9 +9825,9 @@
       <c r="L186">
         <v>0.34705882352941197</v>
       </c>
-      <c r="M186" t="str">
+      <c r="M186" t="e">
         <f t="shared" si="2"/>
-        <v>Rubber and articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
@@ -11569,9 +11337,9 @@
       <c r="L222">
         <v>0.511802127659575</v>
       </c>
-      <c r="M222" t="str">
+      <c r="M222" t="e">
         <f t="shared" si="3"/>
-        <v>Wood and articles of wood; wood charcoal</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="223" spans="1:13" x14ac:dyDescent="0.25">
@@ -11611,9 +11379,9 @@
       <c r="L223">
         <v>0.51357553191489402</v>
       </c>
-      <c r="M223" t="str">
+      <c r="M223" t="e">
         <f t="shared" si="3"/>
-        <v>Wood and articles of wood; wood charcoal</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.25">
@@ -11653,9 +11421,9 @@
       <c r="L224">
         <v>0.51357553191489402</v>
       </c>
-      <c r="M224" t="str">
+      <c r="M224" t="e">
         <f t="shared" si="3"/>
-        <v>Wood and articles of wood; wood charcoal</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="225" spans="1:13" x14ac:dyDescent="0.25">
@@ -11695,9 +11463,9 @@
       <c r="L225">
         <v>0.511802127659575</v>
       </c>
-      <c r="M225" t="str">
+      <c r="M225" t="e">
         <f t="shared" si="3"/>
-        <v>Wood and articles of wood; wood charcoal</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.25">
@@ -11737,9 +11505,9 @@
       <c r="L226">
         <v>0.51357553191489402</v>
       </c>
-      <c r="M226" t="str">
+      <c r="M226" t="e">
         <f t="shared" si="3"/>
-        <v>Wood and articles of wood; wood charcoal</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="227" spans="1:13" x14ac:dyDescent="0.25">
@@ -12409,9 +12177,9 @@
       <c r="L242">
         <v>0.388070618556701</v>
       </c>
-      <c r="M242" t="str">
+      <c r="M242" t="e">
         <f t="shared" si="3"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="243" spans="1:13" x14ac:dyDescent="0.25">
@@ -12451,9 +12219,9 @@
       <c r="L243">
         <v>0.388070618556701</v>
       </c>
-      <c r="M243" t="str">
+      <c r="M243" t="e">
         <f t="shared" si="3"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="244" spans="1:13" x14ac:dyDescent="0.25">
@@ -12493,9 +12261,9 @@
       <c r="L244">
         <v>0.388070618556701</v>
       </c>
-      <c r="M244" t="str">
+      <c r="M244" t="e">
         <f t="shared" si="3"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.25">
@@ -12535,9 +12303,9 @@
       <c r="L245">
         <v>0.388070618556701</v>
       </c>
-      <c r="M245" t="str">
+      <c r="M245" t="e">
         <f t="shared" si="3"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="246" spans="1:13" x14ac:dyDescent="0.25">
@@ -12577,9 +12345,9 @@
       <c r="L246">
         <v>0.388070618556701</v>
       </c>
-      <c r="M246" t="str">
+      <c r="M246" t="e">
         <f t="shared" si="3"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="247" spans="1:13" x14ac:dyDescent="0.25">
@@ -12619,9 +12387,9 @@
       <c r="L247">
         <v>2.5641025641025599E-2</v>
       </c>
-      <c r="M247" t="str">
+      <c r="M247" t="e">
         <f t="shared" si="3"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="248" spans="1:13" x14ac:dyDescent="0.25">
@@ -12661,9 +12429,9 @@
       <c r="L248">
         <v>2.5641025641025599E-2</v>
       </c>
-      <c r="M248" t="str">
+      <c r="M248" t="e">
         <f t="shared" si="3"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.25">
@@ -12703,9 +12471,9 @@
       <c r="L249">
         <v>2.5641025641025599E-2</v>
       </c>
-      <c r="M249" t="str">
+      <c r="M249" t="e">
         <f t="shared" si="3"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.25">
@@ -12745,9 +12513,9 @@
       <c r="L250">
         <v>2.5641025641025599E-2</v>
       </c>
-      <c r="M250" t="str">
+      <c r="M250" t="e">
         <f t="shared" si="3"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.25">
@@ -12787,9 +12555,9 @@
       <c r="L251">
         <v>2.5641025641025599E-2</v>
       </c>
-      <c r="M251" t="str">
+      <c r="M251" t="e">
         <f t="shared" si="3"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.25">
@@ -12829,9 +12597,9 @@
       <c r="L252">
         <v>0.17708333333333301</v>
       </c>
-      <c r="M252" t="str">
+      <c r="M252" t="e">
         <f t="shared" si="3"/>
-        <v>Cereals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.25">
@@ -12871,9 +12639,9 @@
       <c r="L253">
         <v>0.17708333333333301</v>
       </c>
-      <c r="M253" t="str">
+      <c r="M253" t="e">
         <f t="shared" si="3"/>
-        <v>Cereals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="254" spans="1:13" x14ac:dyDescent="0.25">
@@ -12913,9 +12681,9 @@
       <c r="L254">
         <v>0.19791666666666699</v>
       </c>
-      <c r="M254" t="str">
+      <c r="M254" t="e">
         <f t="shared" si="3"/>
-        <v>Cereals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="255" spans="1:13" x14ac:dyDescent="0.25">
@@ -12955,9 +12723,9 @@
       <c r="L255">
         <v>0.17708333333333301</v>
       </c>
-      <c r="M255" t="str">
+      <c r="M255" t="e">
         <f t="shared" si="3"/>
-        <v>Cereals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.25">
@@ -12997,9 +12765,9 @@
       <c r="L256">
         <v>0.17708333333333301</v>
       </c>
-      <c r="M256" t="str">
+      <c r="M256" t="e">
         <f t="shared" si="3"/>
-        <v>Cereals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.25">
@@ -13249,9 +13017,9 @@
       <c r="L262">
         <v>0.19953098591549301</v>
       </c>
-      <c r="M262" t="str">
+      <c r="M262" t="e">
         <f t="shared" si="4"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="263" spans="1:13" x14ac:dyDescent="0.25">
@@ -13291,9 +13059,9 @@
       <c r="L263">
         <v>0.19953098591549301</v>
       </c>
-      <c r="M263" t="str">
+      <c r="M263" t="e">
         <f t="shared" si="4"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="264" spans="1:13" x14ac:dyDescent="0.25">
@@ -13333,9 +13101,9 @@
       <c r="L264">
         <v>0.19953098591549301</v>
       </c>
-      <c r="M264" t="str">
+      <c r="M264" t="e">
         <f t="shared" si="4"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="265" spans="1:13" x14ac:dyDescent="0.25">
@@ -13375,9 +13143,9 @@
       <c r="L265">
         <v>0.19953098591549301</v>
       </c>
-      <c r="M265" t="str">
+      <c r="M265" t="e">
         <f t="shared" si="4"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="266" spans="1:13" x14ac:dyDescent="0.25">
@@ -13417,9 +13185,9 @@
       <c r="L266">
         <v>0.19953098591549301</v>
       </c>
-      <c r="M266" t="str">
+      <c r="M266" t="e">
         <f t="shared" si="4"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.25">
@@ -13459,9 +13227,9 @@
       <c r="L267">
         <v>0.11975039370078699</v>
       </c>
-      <c r="M267" t="str">
+      <c r="M267" t="e">
         <f t="shared" si="4"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.25">
@@ -13501,9 +13269,9 @@
       <c r="L268">
         <v>0.11975039370078699</v>
       </c>
-      <c r="M268" t="str">
+      <c r="M268" t="e">
         <f t="shared" si="4"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.25">
@@ -13543,9 +13311,9 @@
       <c r="L269">
         <v>0.11975039370078699</v>
       </c>
-      <c r="M269" t="str">
+      <c r="M269" t="e">
         <f t="shared" si="4"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.25">
@@ -13585,9 +13353,9 @@
       <c r="L270">
         <v>0.11975039370078699</v>
       </c>
-      <c r="M270" t="str">
+      <c r="M270" t="e">
         <f t="shared" si="4"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="271" spans="1:13" x14ac:dyDescent="0.25">
@@ -13627,9 +13395,9 @@
       <c r="L271">
         <v>0.11975039370078699</v>
       </c>
-      <c r="M271" t="str">
+      <c r="M271" t="e">
         <f t="shared" si="4"/>
-        <v>Vehicles other than railway or tramway rolling-stock, and parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.25">
@@ -13669,9 +13437,9 @@
       <c r="L272">
         <v>0.22258249999999999</v>
       </c>
-      <c r="M272" t="str">
+      <c r="M272" t="e">
         <f t="shared" si="4"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="273" spans="1:13" x14ac:dyDescent="0.25">
@@ -13711,9 +13479,9 @@
       <c r="L273">
         <v>0.22258249999999999</v>
       </c>
-      <c r="M273" t="str">
+      <c r="M273" t="e">
         <f t="shared" si="4"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.25">
@@ -13753,9 +13521,9 @@
       <c r="L274">
         <v>0.22254465909090901</v>
       </c>
-      <c r="M274" t="str">
+      <c r="M274" t="e">
         <f t="shared" si="4"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="275" spans="1:13" x14ac:dyDescent="0.25">
@@ -13795,9 +13563,9 @@
       <c r="L275">
         <v>0.22102318181818201</v>
       </c>
-      <c r="M275" t="str">
+      <c r="M275" t="e">
         <f t="shared" si="4"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.25">
@@ -13837,9 +13605,9 @@
       <c r="L276">
         <v>0.22153454545454501</v>
       </c>
-      <c r="M276" t="str">
+      <c r="M276" t="e">
         <f t="shared" si="4"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.25">
@@ -13879,9 +13647,9 @@
       <c r="L277">
         <v>0.19183958333333301</v>
       </c>
-      <c r="M277" t="str">
+      <c r="M277" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.25">
@@ -13921,9 +13689,9 @@
       <c r="L278">
         <v>0.19183958333333301</v>
       </c>
-      <c r="M278" t="str">
+      <c r="M278" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.25">
@@ -13963,9 +13731,9 @@
       <c r="L279">
         <v>0.19183958333333301</v>
       </c>
-      <c r="M279" t="str">
+      <c r="M279" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="280" spans="1:13" x14ac:dyDescent="0.25">
@@ -14005,9 +13773,9 @@
       <c r="L280">
         <v>0.19183958333333301</v>
       </c>
-      <c r="M280" t="str">
+      <c r="M280" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.25">
@@ -14047,9 +13815,9 @@
       <c r="L281">
         <v>0.19183958333333301</v>
       </c>
-      <c r="M281" t="str">
+      <c r="M281" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.25">
@@ -14089,9 +13857,9 @@
       <c r="L282">
         <v>0.42852058823529399</v>
       </c>
-      <c r="M282" t="str">
+      <c r="M282" t="e">
         <f t="shared" si="4"/>
-        <v>Oil seeds and oleaginous fruits; miscellaneous grains, seeds and fruit; industrial or medical plants; straw and fodder</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.25">
@@ -14131,9 +13899,9 @@
       <c r="L283">
         <v>0.42852058823529399</v>
       </c>
-      <c r="M283" t="str">
+      <c r="M283" t="e">
         <f t="shared" si="4"/>
-        <v>Oil seeds and oleaginous fruits; miscellaneous grains, seeds and fruit; industrial or medical plants; straw and fodder</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="284" spans="1:13" x14ac:dyDescent="0.25">
@@ -14173,9 +13941,9 @@
       <c r="L284">
         <v>0.42852058823529399</v>
       </c>
-      <c r="M284" t="str">
+      <c r="M284" t="e">
         <f t="shared" si="4"/>
-        <v>Oil seeds and oleaginous fruits; miscellaneous grains, seeds and fruit; industrial or medical plants; straw and fodder</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.25">
@@ -14215,9 +13983,9 @@
       <c r="L285">
         <v>0.42852058823529399</v>
       </c>
-      <c r="M285" t="str">
+      <c r="M285" t="e">
         <f t="shared" si="4"/>
-        <v>Oil seeds and oleaginous fruits; miscellaneous grains, seeds and fruit; industrial or medical plants; straw and fodder</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="286" spans="1:13" x14ac:dyDescent="0.25">
@@ -14257,9 +14025,9 @@
       <c r="L286">
         <v>0.42852058823529399</v>
       </c>
-      <c r="M286" t="str">
+      <c r="M286" t="e">
         <f t="shared" si="4"/>
-        <v>Oil seeds and oleaginous fruits; miscellaneous grains, seeds and fruit; industrial or medical plants; straw and fodder</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="287" spans="1:13" x14ac:dyDescent="0.25">
@@ -14719,9 +14487,9 @@
       <c r="L297">
         <v>0.97222222222222199</v>
       </c>
-      <c r="M297" t="str">
+      <c r="M297" t="e">
         <f t="shared" si="4"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="298" spans="1:13" x14ac:dyDescent="0.25">
@@ -14761,9 +14529,9 @@
       <c r="L298">
         <v>0.97222222222222199</v>
       </c>
-      <c r="M298" t="str">
+      <c r="M298" t="e">
         <f t="shared" si="4"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="299" spans="1:13" x14ac:dyDescent="0.25">
@@ -14803,9 +14571,9 @@
       <c r="L299">
         <v>0.97222222222222199</v>
       </c>
-      <c r="M299" t="str">
+      <c r="M299" t="e">
         <f t="shared" si="4"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="300" spans="1:13" x14ac:dyDescent="0.25">
@@ -14845,9 +14613,9 @@
       <c r="L300">
         <v>0.97222222222222199</v>
       </c>
-      <c r="M300" t="str">
+      <c r="M300" t="e">
         <f t="shared" si="4"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="301" spans="1:13" x14ac:dyDescent="0.25">
@@ -14887,9 +14655,9 @@
       <c r="L301">
         <v>0.97222222222222199</v>
       </c>
-      <c r="M301" t="str">
+      <c r="M301" t="e">
         <f t="shared" si="4"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="302" spans="1:13" x14ac:dyDescent="0.25">
@@ -14929,9 +14697,9 @@
       <c r="L302">
         <v>0.727424137931034</v>
       </c>
-      <c r="M302" t="str">
+      <c r="M302" t="e">
         <f t="shared" si="4"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="303" spans="1:13" x14ac:dyDescent="0.25">
@@ -14971,9 +14739,9 @@
       <c r="L303">
         <v>0.727424137931034</v>
       </c>
-      <c r="M303" t="str">
+      <c r="M303" t="e">
         <f t="shared" si="4"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="304" spans="1:13" x14ac:dyDescent="0.25">
@@ -15013,9 +14781,9 @@
       <c r="L304">
         <v>0.727424137931034</v>
       </c>
-      <c r="M304" t="str">
+      <c r="M304" t="e">
         <f t="shared" si="4"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="305" spans="1:13" x14ac:dyDescent="0.25">
@@ -15055,9 +14823,9 @@
       <c r="L305">
         <v>0.727424137931034</v>
       </c>
-      <c r="M305" t="str">
+      <c r="M305" t="e">
         <f t="shared" si="4"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.25">
@@ -15097,9 +14865,9 @@
       <c r="L306">
         <v>0.727424137931034</v>
       </c>
-      <c r="M306" t="str">
+      <c r="M306" t="e">
         <f t="shared" si="4"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="307" spans="1:13" x14ac:dyDescent="0.25">
@@ -15139,9 +14907,9 @@
       <c r="L307">
         <v>0.424017647058823</v>
       </c>
-      <c r="M307" t="str">
+      <c r="M307" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.25">
@@ -15181,9 +14949,9 @@
       <c r="L308">
         <v>0.424017647058823</v>
       </c>
-      <c r="M308" t="str">
+      <c r="M308" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.25">
@@ -15223,9 +14991,9 @@
       <c r="L309">
         <v>0.424017647058823</v>
       </c>
-      <c r="M309" t="str">
+      <c r="M309" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.25">
@@ -15265,9 +15033,9 @@
       <c r="L310">
         <v>0.424017647058823</v>
       </c>
-      <c r="M310" t="str">
+      <c r="M310" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.25">
@@ -15307,9 +15075,9 @@
       <c r="L311">
         <v>0.424017647058823</v>
       </c>
-      <c r="M311" t="str">
+      <c r="M311" t="e">
         <f t="shared" si="4"/>
-        <v>Beverages, spirits and vinegar</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.25">
@@ -15349,9 +15117,9 @@
       <c r="L312">
         <v>0.36904999999999999</v>
       </c>
-      <c r="M312" t="str">
+      <c r="M312" t="e">
         <f t="shared" si="4"/>
-        <v>Animal or vegetable fats and oils and their cleavage products; prepared edible fats; animal or vegetable waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.25">
@@ -15391,9 +15159,9 @@
       <c r="L313">
         <v>0.36904999999999999</v>
       </c>
-      <c r="M313" t="str">
+      <c r="M313" t="e">
         <f t="shared" si="4"/>
-        <v>Animal or vegetable fats and oils and their cleavage products; prepared edible fats; animal or vegetable waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="314" spans="1:13" x14ac:dyDescent="0.25">
@@ -15433,9 +15201,9 @@
       <c r="L314">
         <v>0.36904999999999999</v>
       </c>
-      <c r="M314" t="str">
+      <c r="M314" t="e">
         <f t="shared" si="4"/>
-        <v>Animal or vegetable fats and oils and their cleavage products; prepared edible fats; animal or vegetable waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="315" spans="1:13" x14ac:dyDescent="0.25">
@@ -15475,9 +15243,9 @@
       <c r="L315">
         <v>0.36904999999999999</v>
       </c>
-      <c r="M315" t="str">
+      <c r="M315" t="e">
         <f t="shared" si="4"/>
-        <v>Animal or vegetable fats and oils and their cleavage products; prepared edible fats; animal or vegetable waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="316" spans="1:13" x14ac:dyDescent="0.25">
@@ -15517,9 +15285,9 @@
       <c r="L316">
         <v>0.36904999999999999</v>
       </c>
-      <c r="M316" t="str">
+      <c r="M316" t="e">
         <f t="shared" si="4"/>
-        <v>Animal or vegetable fats and oils and their cleavage products; prepared edible fats; animal or vegetable waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="317" spans="1:13" x14ac:dyDescent="0.25">
@@ -15559,9 +15327,9 @@
       <c r="L317">
         <v>0.21924563492063501</v>
       </c>
-      <c r="M317" t="str">
+      <c r="M317" t="e">
         <f t="shared" si="4"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="318" spans="1:13" x14ac:dyDescent="0.25">
@@ -15601,9 +15369,9 @@
       <c r="L318">
         <v>0.21924563492063501</v>
       </c>
-      <c r="M318" t="str">
+      <c r="M318" t="e">
         <f t="shared" si="4"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="319" spans="1:13" x14ac:dyDescent="0.25">
@@ -15643,9 +15411,9 @@
       <c r="L319">
         <v>0.21924563492063501</v>
       </c>
-      <c r="M319" t="str">
+      <c r="M319" t="e">
         <f t="shared" si="4"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="320" spans="1:13" x14ac:dyDescent="0.25">
@@ -15685,9 +15453,9 @@
       <c r="L320">
         <v>0.21924563492063501</v>
       </c>
-      <c r="M320" t="str">
+      <c r="M320" t="e">
         <f t="shared" si="4"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="321" spans="1:13" x14ac:dyDescent="0.25">
@@ -15727,9 +15495,9 @@
       <c r="L321">
         <v>0.21924563492063501</v>
       </c>
-      <c r="M321" t="str">
+      <c r="M321" t="e">
         <f t="shared" si="4"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="322" spans="1:13" x14ac:dyDescent="0.25">
@@ -16189,9 +15957,9 @@
       <c r="L332">
         <v>1.02040816326531E-2</v>
       </c>
-      <c r="M332" t="str">
+      <c r="M332" t="e">
         <f t="shared" si="5"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.25">
@@ -16231,9 +15999,9 @@
       <c r="L333">
         <v>1.02040816326531E-2</v>
       </c>
-      <c r="M333" t="str">
+      <c r="M333" t="e">
         <f t="shared" si="5"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="334" spans="1:13" x14ac:dyDescent="0.25">
@@ -16273,9 +16041,9 @@
       <c r="L334">
         <v>1.02040816326531E-2</v>
       </c>
-      <c r="M334" t="str">
+      <c r="M334" t="e">
         <f t="shared" si="5"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="335" spans="1:13" x14ac:dyDescent="0.25">
@@ -16315,9 +16083,9 @@
       <c r="L335">
         <v>1.02040816326531E-2</v>
       </c>
-      <c r="M335" t="str">
+      <c r="M335" t="e">
         <f t="shared" si="5"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="336" spans="1:13" x14ac:dyDescent="0.25">
@@ -16357,9 +16125,9 @@
       <c r="L336">
         <v>1.02040816326531E-2</v>
       </c>
-      <c r="M336" t="str">
+      <c r="M336" t="e">
         <f t="shared" si="5"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="337" spans="1:13" x14ac:dyDescent="0.25">
@@ -16399,9 +16167,9 @@
       <c r="L337">
         <v>0.75992222222222205</v>
       </c>
-      <c r="M337" t="str">
+      <c r="M337" t="e">
         <f t="shared" si="5"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.25">
@@ -16441,9 +16209,9 @@
       <c r="L338">
         <v>0.75992222222222205</v>
       </c>
-      <c r="M338" t="str">
+      <c r="M338" t="e">
         <f t="shared" si="5"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.25">
@@ -16483,9 +16251,9 @@
       <c r="L339">
         <v>0.75992222222222205</v>
       </c>
-      <c r="M339" t="str">
+      <c r="M339" t="e">
         <f t="shared" si="5"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="340" spans="1:13" x14ac:dyDescent="0.25">
@@ -16525,9 +16293,9 @@
       <c r="L340">
         <v>0.75992222222222205</v>
       </c>
-      <c r="M340" t="str">
+      <c r="M340" t="e">
         <f t="shared" si="5"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.25">
@@ -16567,9 +16335,9 @@
       <c r="L341">
         <v>0.81547777777777797</v>
       </c>
-      <c r="M341" t="str">
+      <c r="M341" t="e">
         <f t="shared" si="5"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="342" spans="1:13" x14ac:dyDescent="0.25">
@@ -16609,9 +16377,9 @@
       <c r="L342">
         <v>0.179657388316151</v>
       </c>
-      <c r="M342" t="str">
+      <c r="M342" t="e">
         <f t="shared" si="5"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="343" spans="1:13" x14ac:dyDescent="0.25">
@@ -16651,9 +16419,9 @@
       <c r="L343">
         <v>0.179141924398625</v>
       </c>
-      <c r="M343" t="str">
+      <c r="M343" t="e">
         <f t="shared" si="5"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.25">
@@ -16693,9 +16461,9 @@
       <c r="L344">
         <v>0.17927560137456999</v>
       </c>
-      <c r="M344" t="str">
+      <c r="M344" t="e">
         <f t="shared" si="5"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.25">
@@ -16735,9 +16503,9 @@
       <c r="L345">
         <v>0.17996288659793799</v>
       </c>
-      <c r="M345" t="str">
+      <c r="M345" t="e">
         <f t="shared" si="5"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.25">
@@ -16777,9 +16545,9 @@
       <c r="L346">
         <v>0.17996288659793799</v>
       </c>
-      <c r="M346" t="str">
+      <c r="M346" t="e">
         <f t="shared" si="5"/>
-        <v>Organic chemicals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.25">
@@ -17029,9 +16797,9 @@
       <c r="L352">
         <v>0.10833363636363599</v>
       </c>
-      <c r="M352" t="str">
+      <c r="M352" t="e">
         <f t="shared" si="5"/>
-        <v>Other products</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="353" spans="1:13" x14ac:dyDescent="0.25">
@@ -17071,9 +16839,9 @@
       <c r="L353">
         <v>0.11022727272727301</v>
       </c>
-      <c r="M353" t="str">
+      <c r="M353" t="e">
         <f t="shared" si="5"/>
-        <v>Other products</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="354" spans="1:13" x14ac:dyDescent="0.25">
@@ -17113,9 +16881,9 @@
       <c r="L354">
         <v>0.11022727272727301</v>
       </c>
-      <c r="M354" t="str">
+      <c r="M354" t="e">
         <f t="shared" si="5"/>
-        <v>Other products</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="355" spans="1:13" x14ac:dyDescent="0.25">
@@ -17155,9 +16923,9 @@
       <c r="L355">
         <v>0.11022727272727301</v>
       </c>
-      <c r="M355" t="str">
+      <c r="M355" t="e">
         <f t="shared" si="5"/>
-        <v>Other products</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="356" spans="1:13" x14ac:dyDescent="0.25">
@@ -17197,9 +16965,9 @@
       <c r="L356">
         <v>0.10833363636363599</v>
       </c>
-      <c r="M356" t="str">
+      <c r="M356" t="e">
         <f t="shared" si="5"/>
-        <v>Other products</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="357" spans="1:13" x14ac:dyDescent="0.25">
@@ -17449,9 +17217,9 @@
       <c r="L362">
         <v>1</v>
       </c>
-      <c r="M362" t="str">
+      <c r="M362" t="e">
         <f t="shared" si="5"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="363" spans="1:13" x14ac:dyDescent="0.25">
@@ -17491,9 +17259,9 @@
       <c r="L363">
         <v>1</v>
       </c>
-      <c r="M363" t="str">
+      <c r="M363" t="e">
         <f t="shared" si="5"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="364" spans="1:13" x14ac:dyDescent="0.25">
@@ -17533,9 +17301,9 @@
       <c r="L364">
         <v>1</v>
       </c>
-      <c r="M364" t="str">
+      <c r="M364" t="e">
         <f t="shared" si="5"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="365" spans="1:13" x14ac:dyDescent="0.25">
@@ -17575,9 +17343,9 @@
       <c r="L365">
         <v>1</v>
       </c>
-      <c r="M365" t="str">
+      <c r="M365" t="e">
         <f t="shared" si="5"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="366" spans="1:13" x14ac:dyDescent="0.25">
@@ -17617,9 +17385,9 @@
       <c r="L366">
         <v>1</v>
       </c>
-      <c r="M366" t="str">
+      <c r="M366" t="e">
         <f t="shared" si="5"/>
-        <v>Other base metals; cermets; articles thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="367" spans="1:13" x14ac:dyDescent="0.25">
@@ -17659,9 +17427,9 @@
       <c r="L367">
         <v>7.4830612244897995E-2</v>
       </c>
-      <c r="M367" t="str">
+      <c r="M367" t="e">
         <f t="shared" si="5"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="368" spans="1:13" x14ac:dyDescent="0.25">
@@ -17701,9 +17469,9 @@
       <c r="L368">
         <v>7.4830612244897995E-2</v>
       </c>
-      <c r="M368" t="str">
+      <c r="M368" t="e">
         <f t="shared" si="5"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="369" spans="1:13" x14ac:dyDescent="0.25">
@@ -17743,9 +17511,9 @@
       <c r="L369">
         <v>7.4830612244897995E-2</v>
       </c>
-      <c r="M369" t="str">
+      <c r="M369" t="e">
         <f t="shared" si="5"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="370" spans="1:13" x14ac:dyDescent="0.25">
@@ -17785,9 +17553,9 @@
       <c r="L370">
         <v>7.4830612244897995E-2</v>
       </c>
-      <c r="M370" t="str">
+      <c r="M370" t="e">
         <f t="shared" si="5"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="371" spans="1:13" x14ac:dyDescent="0.25">
@@ -17827,9 +17595,9 @@
       <c r="L371">
         <v>7.4830612244897995E-2</v>
       </c>
-      <c r="M371" t="str">
+      <c r="M371" t="e">
         <f t="shared" si="5"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="372" spans="1:13" x14ac:dyDescent="0.25">
@@ -18499,9 +18267,9 @@
       <c r="L387">
         <v>0.18396226415094299</v>
       </c>
-      <c r="M387" t="str">
+      <c r="M387" t="e">
         <f t="shared" ref="M387:M450" si="6">INDEX($P$2:$P$90,MATCH(I387,$O$2:$O$90,0))</f>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="388" spans="1:13" x14ac:dyDescent="0.25">
@@ -18541,9 +18309,9 @@
       <c r="L388">
         <v>0.18396226415094299</v>
       </c>
-      <c r="M388" t="str">
+      <c r="M388" t="e">
         <f t="shared" si="6"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="389" spans="1:13" x14ac:dyDescent="0.25">
@@ -18583,9 +18351,9 @@
       <c r="L389">
         <v>0.18396226415094299</v>
       </c>
-      <c r="M389" t="str">
+      <c r="M389" t="e">
         <f t="shared" si="6"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.25">
@@ -18625,9 +18393,9 @@
       <c r="L390">
         <v>0.18396226415094299</v>
       </c>
-      <c r="M390" t="str">
+      <c r="M390" t="e">
         <f t="shared" si="6"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="391" spans="1:13" x14ac:dyDescent="0.25">
@@ -18667,9 +18435,9 @@
       <c r="L391">
         <v>0.18396226415094299</v>
       </c>
-      <c r="M391" t="str">
+      <c r="M391" t="e">
         <f t="shared" si="6"/>
-        <v>Nuclear reactors, boilers, machinery and mechanical appliances; parts thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="392" spans="1:13" x14ac:dyDescent="0.25">
@@ -18709,9 +18477,9 @@
       <c r="L392">
         <v>0.20433999999999999</v>
       </c>
-      <c r="M392" t="str">
+      <c r="M392" t="e">
         <f t="shared" si="6"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="393" spans="1:13" x14ac:dyDescent="0.25">
@@ -18751,9 +18519,9 @@
       <c r="L393">
         <v>0.20433999999999999</v>
       </c>
-      <c r="M393" t="str">
+      <c r="M393" t="e">
         <f t="shared" si="6"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="394" spans="1:13" x14ac:dyDescent="0.25">
@@ -18793,9 +18561,9 @@
       <c r="L394">
         <v>0.20433999999999999</v>
       </c>
-      <c r="M394" t="str">
+      <c r="M394" t="e">
         <f t="shared" si="6"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="395" spans="1:13" x14ac:dyDescent="0.25">
@@ -18835,9 +18603,9 @@
       <c r="L395">
         <v>0.19633999999999999</v>
       </c>
-      <c r="M395" t="str">
+      <c r="M395" t="e">
         <f t="shared" si="6"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="396" spans="1:13" x14ac:dyDescent="0.25">
@@ -18877,9 +18645,9 @@
       <c r="L396">
         <v>0.19633999999999999</v>
       </c>
-      <c r="M396" t="str">
+      <c r="M396" t="e">
         <f t="shared" si="6"/>
-        <v>Mineral fuels, mineral oils and products of their distillation; bituminous substances; mineral waxes</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="397" spans="1:13" x14ac:dyDescent="0.25">
@@ -19969,9 +19737,9 @@
       <c r="L422">
         <v>0.90625</v>
       </c>
-      <c r="M422" t="str">
+      <c r="M422" t="e">
         <f t="shared" si="6"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="423" spans="1:13" x14ac:dyDescent="0.25">
@@ -20011,9 +19779,9 @@
       <c r="L423">
         <v>0.90625</v>
       </c>
-      <c r="M423" t="str">
+      <c r="M423" t="e">
         <f t="shared" si="6"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="424" spans="1:13" x14ac:dyDescent="0.25">
@@ -20053,9 +19821,9 @@
       <c r="L424">
         <v>0.90625</v>
       </c>
-      <c r="M424" t="str">
+      <c r="M424" t="e">
         <f t="shared" si="6"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="425" spans="1:13" x14ac:dyDescent="0.25">
@@ -20095,9 +19863,9 @@
       <c r="L425">
         <v>0.90625</v>
       </c>
-      <c r="M425" t="str">
+      <c r="M425" t="e">
         <f t="shared" si="6"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="426" spans="1:13" x14ac:dyDescent="0.25">
@@ -20137,9 +19905,9 @@
       <c r="L426">
         <v>0.90625</v>
       </c>
-      <c r="M426" t="str">
+      <c r="M426" t="e">
         <f t="shared" si="6"/>
-        <v>Optical, photographic, cinematographic, measuring, checking, precision, medical or surgical instruments and apparatus; parts and accessories thereof</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="427" spans="1:13" x14ac:dyDescent="0.25">
@@ -20179,9 +19947,9 @@
       <c r="L427">
         <v>5.2181818181818197E-2</v>
       </c>
-      <c r="M427" t="str">
+      <c r="M427" t="e">
         <f t="shared" si="6"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="428" spans="1:13" x14ac:dyDescent="0.25">
@@ -20221,9 +19989,9 @@
       <c r="L428">
         <v>5.2181818181818197E-2</v>
       </c>
-      <c r="M428" t="str">
+      <c r="M428" t="e">
         <f t="shared" si="6"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="429" spans="1:13" x14ac:dyDescent="0.25">
@@ -20263,9 +20031,9 @@
       <c r="L429">
         <v>5.2181818181818197E-2</v>
       </c>
-      <c r="M429" t="str">
+      <c r="M429" t="e">
         <f t="shared" si="6"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="430" spans="1:13" x14ac:dyDescent="0.25">
@@ -20305,9 +20073,9 @@
       <c r="L430">
         <v>5.2181818181818197E-2</v>
       </c>
-      <c r="M430" t="str">
+      <c r="M430" t="e">
         <f t="shared" si="6"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="431" spans="1:13" x14ac:dyDescent="0.25">
@@ -20347,9 +20115,9 @@
       <c r="L431">
         <v>5.2181818181818197E-2</v>
       </c>
-      <c r="M431" t="str">
+      <c r="M431" t="e">
         <f t="shared" si="6"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="432" spans="1:13" x14ac:dyDescent="0.25">
@@ -20389,9 +20157,9 @@
       <c r="L432">
         <v>1</v>
       </c>
-      <c r="M432" t="str">
+      <c r="M432" t="e">
         <f t="shared" si="6"/>
-        <v>Cotton</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="433" spans="1:13" x14ac:dyDescent="0.25">
@@ -20431,9 +20199,9 @@
       <c r="L433">
         <v>1</v>
       </c>
-      <c r="M433" t="str">
+      <c r="M433" t="e">
         <f t="shared" si="6"/>
-        <v>Cotton</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="434" spans="1:13" x14ac:dyDescent="0.25">
@@ -20473,9 +20241,9 @@
       <c r="L434">
         <v>1</v>
       </c>
-      <c r="M434" t="str">
+      <c r="M434" t="e">
         <f t="shared" si="6"/>
-        <v>Cotton</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="435" spans="1:13" x14ac:dyDescent="0.25">
@@ -20515,9 +20283,9 @@
       <c r="L435">
         <v>1</v>
       </c>
-      <c r="M435" t="str">
+      <c r="M435" t="e">
         <f t="shared" si="6"/>
-        <v>Cotton</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="436" spans="1:13" x14ac:dyDescent="0.25">
@@ -20557,9 +20325,9 @@
       <c r="L436">
         <v>1</v>
       </c>
-      <c r="M436" t="str">
+      <c r="M436" t="e">
         <f t="shared" si="6"/>
-        <v>Cotton</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="437" spans="1:13" x14ac:dyDescent="0.25">
@@ -20599,9 +20367,9 @@
       <c r="L437">
         <v>0.55637058823529395</v>
       </c>
-      <c r="M437" t="str">
+      <c r="M437" t="e">
         <f t="shared" si="6"/>
-        <v>Live animals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="438" spans="1:13" x14ac:dyDescent="0.25">
@@ -20641,9 +20409,9 @@
       <c r="L438">
         <v>0.553920588235294</v>
       </c>
-      <c r="M438" t="str">
+      <c r="M438" t="e">
         <f t="shared" si="6"/>
-        <v>Live animals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="439" spans="1:13" x14ac:dyDescent="0.25">
@@ -20683,9 +20451,9 @@
       <c r="L439">
         <v>0.55637058823529395</v>
       </c>
-      <c r="M439" t="str">
+      <c r="M439" t="e">
         <f t="shared" si="6"/>
-        <v>Live animals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="440" spans="1:13" x14ac:dyDescent="0.25">
@@ -20725,9 +20493,9 @@
       <c r="L440">
         <v>0.55637058823529395</v>
       </c>
-      <c r="M440" t="str">
+      <c r="M440" t="e">
         <f t="shared" si="6"/>
-        <v>Live animals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="441" spans="1:13" x14ac:dyDescent="0.25">
@@ -20767,9 +20535,9 @@
       <c r="L441">
         <v>0.55637058823529395</v>
       </c>
-      <c r="M441" t="str">
+      <c r="M441" t="e">
         <f t="shared" si="6"/>
-        <v>Live animals</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="442" spans="1:13" x14ac:dyDescent="0.25">
@@ -21439,9 +21207,9 @@
       <c r="L457">
         <v>0.39285714285714302</v>
       </c>
-      <c r="M457" t="str">
+      <c r="M457" t="e">
         <f t="shared" si="7"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="458" spans="1:13" x14ac:dyDescent="0.25">
@@ -21481,9 +21249,9 @@
       <c r="L458">
         <v>0.39285714285714302</v>
       </c>
-      <c r="M458" t="str">
+      <c r="M458" t="e">
         <f t="shared" si="7"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="459" spans="1:13" x14ac:dyDescent="0.25">
@@ -21523,9 +21291,9 @@
       <c r="L459">
         <v>0.39285714285714302</v>
       </c>
-      <c r="M459" t="str">
+      <c r="M459" t="e">
         <f t="shared" si="7"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="460" spans="1:13" x14ac:dyDescent="0.25">
@@ -21565,9 +21333,9 @@
       <c r="L460">
         <v>0.39285714285714302</v>
       </c>
-      <c r="M460" t="str">
+      <c r="M460" t="e">
         <f t="shared" si="7"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="461" spans="1:13" x14ac:dyDescent="0.25">
@@ -21607,9 +21375,9 @@
       <c r="L461">
         <v>0.39285714285714302</v>
       </c>
-      <c r="M461" t="str">
+      <c r="M461" t="e">
         <f t="shared" si="7"/>
-        <v>Coffee, tea, mate and spices</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="462" spans="1:13" x14ac:dyDescent="0.25">
@@ -21859,9 +21627,9 @@
       <c r="L467">
         <v>0.39866800000000002</v>
       </c>
-      <c r="M467" t="str">
+      <c r="M467" t="e">
         <f t="shared" si="7"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="468" spans="1:13" x14ac:dyDescent="0.25">
@@ -21901,9 +21669,9 @@
       <c r="L468">
         <v>0.39866800000000002</v>
       </c>
-      <c r="M468" t="str">
+      <c r="M468" t="e">
         <f t="shared" si="7"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="469" spans="1:13" x14ac:dyDescent="0.25">
@@ -21943,9 +21711,9 @@
       <c r="L469">
         <v>0.39866800000000002</v>
       </c>
-      <c r="M469" t="str">
+      <c r="M469" t="e">
         <f t="shared" si="7"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="470" spans="1:13" x14ac:dyDescent="0.25">
@@ -21985,9 +21753,9 @@
       <c r="L470">
         <v>0.39866800000000002</v>
       </c>
-      <c r="M470" t="str">
+      <c r="M470" t="e">
         <f t="shared" si="7"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="471" spans="1:13" x14ac:dyDescent="0.25">
@@ -22027,18 +21795,483 @@
       <c r="L471">
         <v>0.39866800000000002</v>
       </c>
-      <c r="M471" t="str">
+      <c r="M471" t="e">
         <f t="shared" si="7"/>
-        <v>Electrical machinery and equipment and parts thereof; sound recorders and reproducers, television image and sound recorders and reproducers, and parts and accessories of such articles</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M471" xr:uid="{2CA24C76-3D75-422A-B7CD-C37446D883C9}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL&amp;1#_x000D_</oddHeader>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB05E758-CA88-4E80-A5E6-ADD64CF8907B}">
+  <dimension ref="A1:B56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>194</v>
+      </c>
+      <c r="B55" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>198</v>
+      </c>
+      <c r="B56" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>